<commit_message>
critíca 14 do 376 removido
</commit_message>
<xml_diff>
--- a/Excel Models/Insurance/376.xlsx
+++ b/Excel Models/Insurance/376.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcelo.franceschini\OneDrive - GRANT THORNTON BRASIL\MMF\Python\ActuarialServices\Excel Models\Insurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A37F3D95-2A58-466F-AA08-8EBAC0CF166A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{6768FC10-513F-4C8B-9D89-9C5A17DFD2BB}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{A37F3D95-2A58-466F-AA08-8EBAC0CF166A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{50C46735-95DB-49A7-9F4B-0B7362EC1DAC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6D37E46F-5577-46BE-BC57-308DF90C1D4E}"/>
   </bookViews>
@@ -16,71 +16,71 @@
     <sheet name="Validação 376" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="0">'Validação 376'!$A$57</definedName>
-    <definedName name="DadosExternos_10" localSheetId="0">'Validação 376'!$A$77</definedName>
-    <definedName name="DadosExternos_11" localSheetId="0">'Validação 376'!$A$79</definedName>
-    <definedName name="DadosExternos_12" localSheetId="0">'Validação 376'!$A$81</definedName>
-    <definedName name="DadosExternos_13" localSheetId="0">'Validação 376'!$A$83</definedName>
-    <definedName name="DadosExternos_14" localSheetId="0">'Validação 376'!$A$85</definedName>
-    <definedName name="DadosExternos_15" localSheetId="0">'Validação 376'!$A$87</definedName>
-    <definedName name="DadosExternos_16" localSheetId="0">'Validação 376'!$A$89</definedName>
-    <definedName name="DadosExternos_17" localSheetId="0">'Validação 376'!$A$91</definedName>
-    <definedName name="DadosExternos_19" localSheetId="0">'Validação 376'!$A$95</definedName>
-    <definedName name="DadosExternos_2" localSheetId="0">'Validação 376'!$A$61</definedName>
-    <definedName name="DadosExternos_20" localSheetId="0">'Validação 376'!$A$97</definedName>
-    <definedName name="DadosExternos_21" localSheetId="0">'Validação 376'!$A$99</definedName>
-    <definedName name="DadosExternos_22" localSheetId="0">'Validação 376'!$A$101</definedName>
-    <definedName name="DadosExternos_23" localSheetId="0">'Validação 376'!$A$103</definedName>
-    <definedName name="DadosExternos_24" localSheetId="0">'Validação 376'!$A$105</definedName>
-    <definedName name="DadosExternos_25" localSheetId="0">'Validação 376'!$A$107</definedName>
-    <definedName name="DadosExternos_26" localSheetId="0">'Validação 376'!$A$109</definedName>
-    <definedName name="DadosExternos_27" localSheetId="0">'Validação 376'!$A$111</definedName>
-    <definedName name="DadosExternos_28" localSheetId="0">'Validação 376'!$A$113</definedName>
-    <definedName name="DadosExternos_29" localSheetId="0">'Validação 376'!$A$115</definedName>
-    <definedName name="DadosExternos_3" localSheetId="0">'Validação 376'!$A$63</definedName>
-    <definedName name="DadosExternos_30" localSheetId="0">'Validação 376'!$A$117</definedName>
-    <definedName name="DadosExternos_31" localSheetId="0">'Validação 376'!$A$119</definedName>
-    <definedName name="DadosExternos_32" localSheetId="0">'Validação 376'!$A$121</definedName>
-    <definedName name="DadosExternos_34" localSheetId="0">'Validação 376'!$A$125</definedName>
-    <definedName name="DadosExternos_35" localSheetId="0">'Validação 376'!$A$127</definedName>
-    <definedName name="DadosExternos_37" localSheetId="0">'Validação 376'!$A$131</definedName>
-    <definedName name="DadosExternos_38" localSheetId="0">'Validação 376'!$A$133</definedName>
-    <definedName name="DadosExternos_39" localSheetId="0">'Validação 376'!$A$135</definedName>
-    <definedName name="DadosExternos_4" localSheetId="0">'Validação 376'!$A$65</definedName>
-    <definedName name="DadosExternos_40" localSheetId="0">'Validação 376'!$A$137</definedName>
-    <definedName name="DadosExternos_41" localSheetId="0">'Validação 376'!$A$139</definedName>
-    <definedName name="DadosExternos_42" localSheetId="0">'Validação 376'!$A$141</definedName>
-    <definedName name="DadosExternos_43" localSheetId="0">'Validação 376'!$A$143</definedName>
-    <definedName name="DadosExternos_44" localSheetId="0">'Validação 376'!$A$145</definedName>
-    <definedName name="DadosExternos_45" localSheetId="0">'Validação 376'!$A$147</definedName>
-    <definedName name="DadosExternos_46" localSheetId="0">'Validação 376'!$A$149</definedName>
-    <definedName name="DadosExternos_47" localSheetId="0">'Validação 376'!$A$151</definedName>
-    <definedName name="DadosExternos_48" localSheetId="0">'Validação 376'!$A$153</definedName>
-    <definedName name="DadosExternos_49" localSheetId="0">'Validação 376'!$A$155</definedName>
-    <definedName name="DadosExternos_5" localSheetId="0">'Validação 376'!$A$67</definedName>
-    <definedName name="DadosExternos_50" localSheetId="0">'Validação 376'!$A$157</definedName>
-    <definedName name="DadosExternos_51" localSheetId="0">'Validação 376'!$A$159</definedName>
-    <definedName name="DadosExternos_53" localSheetId="0">'Validação 376'!$A$163</definedName>
-    <definedName name="DadosExternos_54" localSheetId="0">'Validação 376'!$A$165</definedName>
-    <definedName name="DadosExternos_55" localSheetId="0">'Validação 376'!$A$167</definedName>
-    <definedName name="DadosExternos_56" localSheetId="0">'Validação 376'!$A$169</definedName>
-    <definedName name="DadosExternos_57" localSheetId="0">'Validação 376'!$A$171</definedName>
-    <definedName name="DadosExternos_59" localSheetId="0">'Validação 376'!$A$175</definedName>
-    <definedName name="DadosExternos_6" localSheetId="0">'Validação 376'!$A$69</definedName>
-    <definedName name="DadosExternos_60" localSheetId="0">'Validação 376'!$A$177</definedName>
-    <definedName name="DadosExternos_61" localSheetId="0">'Validação 376'!$A$179</definedName>
-    <definedName name="DadosExternos_62" localSheetId="0">'Validação 376'!$A$181</definedName>
-    <definedName name="DadosExternos_63" localSheetId="0">'Validação 376'!$A$183</definedName>
-    <definedName name="DadosExternos_64" localSheetId="0">'Validação 376'!$A$185</definedName>
-    <definedName name="DadosExternos_65" localSheetId="0">'Validação 376'!$A$187</definedName>
-    <definedName name="DadosExternos_66" localSheetId="0">'Validação 376'!$A$189</definedName>
-    <definedName name="DadosExternos_67" localSheetId="0">'Validação 376'!$A$191</definedName>
-    <definedName name="DadosExternos_68" localSheetId="0">'Validação 376'!$A$193</definedName>
-    <definedName name="DadosExternos_69" localSheetId="0">'Validação 376'!$A$195</definedName>
-    <definedName name="DadosExternos_7" localSheetId="0">'Validação 376'!$A$71</definedName>
-    <definedName name="DadosExternos_70" localSheetId="0">'Validação 376'!$A$197</definedName>
-    <definedName name="DadosExternos_8" localSheetId="0">'Validação 376'!$A$73</definedName>
-    <definedName name="DadosExternos_9" localSheetId="0">'Validação 376'!$A$75</definedName>
+    <definedName name="DadosExternos_1" localSheetId="0">'Validação 376'!$A$56</definedName>
+    <definedName name="DadosExternos_10" localSheetId="0">'Validação 376'!$A$76</definedName>
+    <definedName name="DadosExternos_11" localSheetId="0">'Validação 376'!$A$78</definedName>
+    <definedName name="DadosExternos_12" localSheetId="0">'Validação 376'!$A$80</definedName>
+    <definedName name="DadosExternos_13" localSheetId="0">'Validação 376'!$A$82</definedName>
+    <definedName name="DadosExternos_14" localSheetId="0">'Validação 376'!$A$84</definedName>
+    <definedName name="DadosExternos_15" localSheetId="0">'Validação 376'!$A$86</definedName>
+    <definedName name="DadosExternos_16" localSheetId="0">'Validação 376'!$A$88</definedName>
+    <definedName name="DadosExternos_17" localSheetId="0">'Validação 376'!$A$90</definedName>
+    <definedName name="DadosExternos_19" localSheetId="0">'Validação 376'!$A$94</definedName>
+    <definedName name="DadosExternos_2" localSheetId="0">'Validação 376'!$A$60</definedName>
+    <definedName name="DadosExternos_20" localSheetId="0">'Validação 376'!$A$96</definedName>
+    <definedName name="DadosExternos_21" localSheetId="0">'Validação 376'!$A$98</definedName>
+    <definedName name="DadosExternos_22" localSheetId="0">'Validação 376'!$A$100</definedName>
+    <definedName name="DadosExternos_23" localSheetId="0">'Validação 376'!$A$102</definedName>
+    <definedName name="DadosExternos_24" localSheetId="0">'Validação 376'!$A$104</definedName>
+    <definedName name="DadosExternos_25" localSheetId="0">'Validação 376'!$A$106</definedName>
+    <definedName name="DadosExternos_26" localSheetId="0">'Validação 376'!$A$108</definedName>
+    <definedName name="DadosExternos_27" localSheetId="0">'Validação 376'!$A$110</definedName>
+    <definedName name="DadosExternos_28" localSheetId="0">'Validação 376'!$A$112</definedName>
+    <definedName name="DadosExternos_29" localSheetId="0">'Validação 376'!$A$114</definedName>
+    <definedName name="DadosExternos_3" localSheetId="0">'Validação 376'!$A$62</definedName>
+    <definedName name="DadosExternos_30" localSheetId="0">'Validação 376'!$A$116</definedName>
+    <definedName name="DadosExternos_31" localSheetId="0">'Validação 376'!$A$118</definedName>
+    <definedName name="DadosExternos_32" localSheetId="0">'Validação 376'!$A$120</definedName>
+    <definedName name="DadosExternos_34" localSheetId="0">'Validação 376'!$A$124</definedName>
+    <definedName name="DadosExternos_35" localSheetId="0">'Validação 376'!$A$126</definedName>
+    <definedName name="DadosExternos_37" localSheetId="0">'Validação 376'!$A$130</definedName>
+    <definedName name="DadosExternos_38" localSheetId="0">'Validação 376'!$A$132</definedName>
+    <definedName name="DadosExternos_39" localSheetId="0">'Validação 376'!$A$134</definedName>
+    <definedName name="DadosExternos_4" localSheetId="0">'Validação 376'!$A$64</definedName>
+    <definedName name="DadosExternos_40" localSheetId="0">'Validação 376'!$A$136</definedName>
+    <definedName name="DadosExternos_41" localSheetId="0">'Validação 376'!$A$138</definedName>
+    <definedName name="DadosExternos_42" localSheetId="0">'Validação 376'!$A$140</definedName>
+    <definedName name="DadosExternos_43" localSheetId="0">'Validação 376'!$A$142</definedName>
+    <definedName name="DadosExternos_44" localSheetId="0">'Validação 376'!$A$144</definedName>
+    <definedName name="DadosExternos_45" localSheetId="0">'Validação 376'!$A$146</definedName>
+    <definedName name="DadosExternos_46" localSheetId="0">'Validação 376'!$A$148</definedName>
+    <definedName name="DadosExternos_47" localSheetId="0">'Validação 376'!$A$150</definedName>
+    <definedName name="DadosExternos_48" localSheetId="0">'Validação 376'!$A$152</definedName>
+    <definedName name="DadosExternos_49" localSheetId="0">'Validação 376'!$A$154</definedName>
+    <definedName name="DadosExternos_5" localSheetId="0">'Validação 376'!$A$66</definedName>
+    <definedName name="DadosExternos_50" localSheetId="0">'Validação 376'!$A$156</definedName>
+    <definedName name="DadosExternos_51" localSheetId="0">'Validação 376'!$A$158</definedName>
+    <definedName name="DadosExternos_53" localSheetId="0">'Validação 376'!$A$162</definedName>
+    <definedName name="DadosExternos_54" localSheetId="0">'Validação 376'!$A$164</definedName>
+    <definedName name="DadosExternos_55" localSheetId="0">'Validação 376'!$A$166</definedName>
+    <definedName name="DadosExternos_56" localSheetId="0">'Validação 376'!$A$168</definedName>
+    <definedName name="DadosExternos_57" localSheetId="0">'Validação 376'!$A$170</definedName>
+    <definedName name="DadosExternos_59" localSheetId="0">'Validação 376'!$A$174</definedName>
+    <definedName name="DadosExternos_6" localSheetId="0">'Validação 376'!$A$68</definedName>
+    <definedName name="DadosExternos_60" localSheetId="0">'Validação 376'!$A$176</definedName>
+    <definedName name="DadosExternos_61" localSheetId="0">'Validação 376'!$A$178</definedName>
+    <definedName name="DadosExternos_62" localSheetId="0">'Validação 376'!$A$180</definedName>
+    <definedName name="DadosExternos_63" localSheetId="0">'Validação 376'!$A$182</definedName>
+    <definedName name="DadosExternos_64" localSheetId="0">'Validação 376'!$A$184</definedName>
+    <definedName name="DadosExternos_65" localSheetId="0">'Validação 376'!$A$186</definedName>
+    <definedName name="DadosExternos_66" localSheetId="0">'Validação 376'!$A$188</definedName>
+    <definedName name="DadosExternos_67" localSheetId="0">'Validação 376'!$A$190</definedName>
+    <definedName name="DadosExternos_68" localSheetId="0">'Validação 376'!$A$192</definedName>
+    <definedName name="DadosExternos_69" localSheetId="0">'Validação 376'!$A$194</definedName>
+    <definedName name="DadosExternos_7" localSheetId="0">'Validação 376'!$A$70</definedName>
+    <definedName name="DadosExternos_70" localSheetId="0">'Validação 376'!$A$196</definedName>
+    <definedName name="DadosExternos_8" localSheetId="0">'Validação 376'!$A$72</definedName>
+    <definedName name="DadosExternos_9" localSheetId="0">'Validação 376'!$A$74</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="40">
   <si>
     <t>GRANT THORNTON SERVIÇOS ATUARIAIS</t>
   </si>
@@ -239,9 +239,6 @@
   <si>
     <t>TOTAL</t>
   </si>
-  <si>
-    <t>#14</t>
-  </si>
 </sst>
 </file>
 
@@ -322,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -608,51 +605,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -715,7 +667,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -778,29 +730,22 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -815,6 +760,12 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,12 +773,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,13 +957,13 @@
       <xdr:col>81</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>89</xdr:col>
       <xdr:colOff>151699</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>190364</xdr:rowOff>
+      <xdr:rowOff>133214</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1354,11 +1299,13 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:CL33"/>
+  <dimension ref="A1:CL32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:I26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
@@ -1399,7 +1346,7 @@
     <row r="2" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:89" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:89" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,123 +1395,123 @@
     </row>
     <row r="11" spans="2:89" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:89" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
-      <c r="M12" s="39" t="s">
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
+      <c r="M12" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="41"/>
-      <c r="S12" s="39" t="s">
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="40"/>
+      <c r="S12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="T12" s="40"/>
-      <c r="U12" s="40"/>
-      <c r="V12" s="40"/>
-      <c r="W12" s="41"/>
-      <c r="Y12" s="39" t="s">
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="40"/>
+      <c r="Y12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="Z12" s="40"/>
-      <c r="AA12" s="40"/>
-      <c r="AB12" s="40"/>
-      <c r="AC12" s="41"/>
-      <c r="AE12" s="39" t="s">
+      <c r="Z12" s="39"/>
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="40"/>
+      <c r="AE12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AF12" s="40"/>
-      <c r="AG12" s="40"/>
-      <c r="AH12" s="40"/>
-      <c r="AI12" s="41"/>
-      <c r="AK12" s="39" t="s">
+      <c r="AF12" s="39"/>
+      <c r="AG12" s="39"/>
+      <c r="AH12" s="39"/>
+      <c r="AI12" s="40"/>
+      <c r="AK12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AL12" s="40"/>
-      <c r="AM12" s="40"/>
-      <c r="AN12" s="40"/>
-      <c r="AO12" s="41"/>
-      <c r="AQ12" s="39" t="s">
+      <c r="AL12" s="39"/>
+      <c r="AM12" s="39"/>
+      <c r="AN12" s="39"/>
+      <c r="AO12" s="40"/>
+      <c r="AQ12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AR12" s="40"/>
-      <c r="AS12" s="40"/>
-      <c r="AT12" s="40"/>
-      <c r="AU12" s="41"/>
-      <c r="AW12" s="39" t="s">
+      <c r="AR12" s="39"/>
+      <c r="AS12" s="39"/>
+      <c r="AT12" s="39"/>
+      <c r="AU12" s="40"/>
+      <c r="AW12" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="AX12" s="40"/>
-      <c r="AY12" s="40"/>
-      <c r="AZ12" s="40"/>
-      <c r="BA12" s="41"/>
-      <c r="BC12" s="39" t="s">
+      <c r="AX12" s="39"/>
+      <c r="AY12" s="39"/>
+      <c r="AZ12" s="39"/>
+      <c r="BA12" s="40"/>
+      <c r="BC12" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="BD12" s="40"/>
-      <c r="BE12" s="40"/>
-      <c r="BF12" s="40"/>
-      <c r="BG12" s="41"/>
-      <c r="BI12" s="39" t="s">
+      <c r="BD12" s="39"/>
+      <c r="BE12" s="39"/>
+      <c r="BF12" s="39"/>
+      <c r="BG12" s="40"/>
+      <c r="BI12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="BJ12" s="40"/>
-      <c r="BK12" s="40"/>
-      <c r="BL12" s="40"/>
-      <c r="BM12" s="41"/>
-      <c r="BO12" s="39" t="s">
+      <c r="BJ12" s="39"/>
+      <c r="BK12" s="39"/>
+      <c r="BL12" s="39"/>
+      <c r="BM12" s="40"/>
+      <c r="BO12" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="BP12" s="40"/>
-      <c r="BQ12" s="40"/>
-      <c r="BR12" s="40"/>
-      <c r="BS12" s="41"/>
-      <c r="BU12" s="39" t="s">
+      <c r="BP12" s="39"/>
+      <c r="BQ12" s="39"/>
+      <c r="BR12" s="39"/>
+      <c r="BS12" s="40"/>
+      <c r="BU12" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="BV12" s="40"/>
-      <c r="BW12" s="40"/>
-      <c r="BX12" s="40"/>
-      <c r="BY12" s="41"/>
-      <c r="CA12" s="39" t="s">
+      <c r="BV12" s="39"/>
+      <c r="BW12" s="39"/>
+      <c r="BX12" s="39"/>
+      <c r="BY12" s="40"/>
+      <c r="CA12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="CB12" s="40"/>
-      <c r="CC12" s="40"/>
-      <c r="CD12" s="40"/>
-      <c r="CE12" s="41"/>
-      <c r="CG12" s="39" t="s">
+      <c r="CB12" s="39"/>
+      <c r="CC12" s="39"/>
+      <c r="CD12" s="39"/>
+      <c r="CE12" s="40"/>
+      <c r="CG12" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="CH12" s="40"/>
-      <c r="CI12" s="40"/>
-      <c r="CJ12" s="40"/>
-      <c r="CK12" s="41"/>
+      <c r="CH12" s="39"/>
+      <c r="CI12" s="39"/>
+      <c r="CJ12" s="39"/>
+      <c r="CK12" s="40"/>
     </row>
     <row r="13" spans="2:89" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="31" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -1793,7 +1740,7 @@
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="35">
+      <c r="J14" s="32">
         <f>H14-I14</f>
         <v>0</v>
       </c>
@@ -1806,7 +1753,7 @@
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
-      <c r="P14" s="35">
+      <c r="P14" s="32">
         <f>N14-O14</f>
         <v>0</v>
       </c>
@@ -1819,7 +1766,7 @@
       </c>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
-      <c r="V14" s="35">
+      <c r="V14" s="32">
         <f>T14-U14</f>
         <v>0</v>
       </c>
@@ -1832,7 +1779,7 @@
       </c>
       <c r="Z14" s="14"/>
       <c r="AA14" s="14"/>
-      <c r="AB14" s="35">
+      <c r="AB14" s="32">
         <f>Z14-AA14</f>
         <v>0</v>
       </c>
@@ -1845,7 +1792,7 @@
       </c>
       <c r="AF14" s="14"/>
       <c r="AG14" s="14"/>
-      <c r="AH14" s="35">
+      <c r="AH14" s="32">
         <f>AF14-AG14</f>
         <v>0</v>
       </c>
@@ -1858,7 +1805,7 @@
       </c>
       <c r="AL14" s="14"/>
       <c r="AM14" s="14"/>
-      <c r="AN14" s="35">
+      <c r="AN14" s="32">
         <f>AL14-AM14</f>
         <v>0</v>
       </c>
@@ -1871,7 +1818,7 @@
       </c>
       <c r="AR14" s="14"/>
       <c r="AS14" s="14"/>
-      <c r="AT14" s="35">
+      <c r="AT14" s="32">
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
@@ -1884,7 +1831,7 @@
       </c>
       <c r="AX14" s="14"/>
       <c r="AY14" s="14"/>
-      <c r="AZ14" s="35">
+      <c r="AZ14" s="32">
         <f>AX14-AY14</f>
         <v>0</v>
       </c>
@@ -1897,7 +1844,7 @@
       </c>
       <c r="BD14" s="14"/>
       <c r="BE14" s="14"/>
-      <c r="BF14" s="35">
+      <c r="BF14" s="32">
         <f>BD14-BE14</f>
         <v>0</v>
       </c>
@@ -1910,7 +1857,7 @@
       </c>
       <c r="BJ14" s="14"/>
       <c r="BK14" s="14"/>
-      <c r="BL14" s="35">
+      <c r="BL14" s="32">
         <f>BJ14-BK14</f>
         <v>0</v>
       </c>
@@ -1923,7 +1870,7 @@
       </c>
       <c r="BP14" s="14"/>
       <c r="BQ14" s="14"/>
-      <c r="BR14" s="35">
+      <c r="BR14" s="32">
         <f>BP14-BQ14</f>
         <v>0</v>
       </c>
@@ -1936,7 +1883,7 @@
       </c>
       <c r="BV14" s="14"/>
       <c r="BW14" s="14"/>
-      <c r="BX14" s="35">
+      <c r="BX14" s="32">
         <f>BV14-BW14</f>
         <v>0</v>
       </c>
@@ -1949,7 +1896,7 @@
       </c>
       <c r="CB14" s="14"/>
       <c r="CC14" s="14"/>
-      <c r="CD14" s="35">
+      <c r="CD14" s="32">
         <f>CB14-CC14</f>
         <v>0</v>
       </c>
@@ -1962,7 +1909,7 @@
       </c>
       <c r="CH14" s="14"/>
       <c r="CI14" s="14"/>
-      <c r="CJ14" s="35">
+      <c r="CJ14" s="32">
         <f>CH14-CI14</f>
         <v>0</v>
       </c>
@@ -1978,7 +1925,7 @@
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="18">
-        <f t="shared" ref="E15:E27" si="0">IF(ISERR(D15/C15),,(D15/C15))</f>
+        <f t="shared" ref="E15:E26" si="0">IF(ISERR(D15/C15),,(D15/C15))</f>
         <v>0</v>
       </c>
       <c r="G15" s="19">
@@ -1986,7 +1933,7 @@
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="36">
+      <c r="J15" s="33">
         <f t="shared" ref="J15:J25" si="1">H15-I15</f>
         <v>0</v>
       </c>
@@ -1999,7 +1946,7 @@
       </c>
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
-      <c r="P15" s="36">
+      <c r="P15" s="33">
         <f t="shared" ref="P15:P25" si="3">N15-O15</f>
         <v>0</v>
       </c>
@@ -2012,7 +1959,7 @@
       </c>
       <c r="T15" s="20"/>
       <c r="U15" s="20"/>
-      <c r="V15" s="36">
+      <c r="V15" s="33">
         <f t="shared" ref="V15:V25" si="5">T15-U15</f>
         <v>0</v>
       </c>
@@ -2025,7 +1972,7 @@
       </c>
       <c r="Z15" s="20"/>
       <c r="AA15" s="20"/>
-      <c r="AB15" s="36">
+      <c r="AB15" s="33">
         <f t="shared" ref="AB15:AB25" si="7">Z15-AA15</f>
         <v>0</v>
       </c>
@@ -2038,7 +1985,7 @@
       </c>
       <c r="AF15" s="20"/>
       <c r="AG15" s="20"/>
-      <c r="AH15" s="36">
+      <c r="AH15" s="33">
         <f t="shared" ref="AH15:AH25" si="9">AF15-AG15</f>
         <v>0</v>
       </c>
@@ -2051,7 +1998,7 @@
       </c>
       <c r="AL15" s="20"/>
       <c r="AM15" s="20"/>
-      <c r="AN15" s="36">
+      <c r="AN15" s="33">
         <f t="shared" ref="AN15:AN25" si="11">AL15-AM15</f>
         <v>0</v>
       </c>
@@ -2064,7 +2011,7 @@
       </c>
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
-      <c r="AT15" s="36">
+      <c r="AT15" s="33">
         <f t="shared" ref="AT15:AT25" si="13">AR15-AS15</f>
         <v>0</v>
       </c>
@@ -2077,7 +2024,7 @@
       </c>
       <c r="AX15" s="20"/>
       <c r="AY15" s="20"/>
-      <c r="AZ15" s="36">
+      <c r="AZ15" s="33">
         <f t="shared" ref="AZ15:AZ25" si="15">AX15-AY15</f>
         <v>0</v>
       </c>
@@ -2090,7 +2037,7 @@
       </c>
       <c r="BD15" s="20"/>
       <c r="BE15" s="20"/>
-      <c r="BF15" s="36">
+      <c r="BF15" s="33">
         <f t="shared" ref="BF15:BF25" si="17">BD15-BE15</f>
         <v>0</v>
       </c>
@@ -2103,7 +2050,7 @@
       </c>
       <c r="BJ15" s="20"/>
       <c r="BK15" s="20"/>
-      <c r="BL15" s="36">
+      <c r="BL15" s="33">
         <f t="shared" ref="BL15:BL25" si="19">BJ15-BK15</f>
         <v>0</v>
       </c>
@@ -2116,7 +2063,7 @@
       </c>
       <c r="BP15" s="20"/>
       <c r="BQ15" s="20"/>
-      <c r="BR15" s="36">
+      <c r="BR15" s="33">
         <f t="shared" ref="BR15:BR25" si="21">BP15-BQ15</f>
         <v>0</v>
       </c>
@@ -2129,7 +2076,7 @@
       </c>
       <c r="BV15" s="20"/>
       <c r="BW15" s="20"/>
-      <c r="BX15" s="36">
+      <c r="BX15" s="33">
         <f t="shared" ref="BX15:BX25" si="23">BV15-BW15</f>
         <v>0</v>
       </c>
@@ -2142,7 +2089,7 @@
       </c>
       <c r="CB15" s="20"/>
       <c r="CC15" s="20"/>
-      <c r="CD15" s="36">
+      <c r="CD15" s="33">
         <f t="shared" ref="CD15:CD25" si="25">CB15-CC15</f>
         <v>0</v>
       </c>
@@ -2155,7 +2102,7 @@
       </c>
       <c r="CH15" s="20"/>
       <c r="CI15" s="20"/>
-      <c r="CJ15" s="36">
+      <c r="CJ15" s="33">
         <f t="shared" ref="CJ15:CJ25" si="27">CH15-CI15</f>
         <v>0</v>
       </c>
@@ -2179,7 +2126,7 @@
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
-      <c r="J16" s="36">
+      <c r="J16" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2192,7 +2139,7 @@
       </c>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
-      <c r="P16" s="36">
+      <c r="P16" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2205,7 +2152,7 @@
       </c>
       <c r="T16" s="20"/>
       <c r="U16" s="20"/>
-      <c r="V16" s="36">
+      <c r="V16" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2218,7 +2165,7 @@
       </c>
       <c r="Z16" s="20"/>
       <c r="AA16" s="20"/>
-      <c r="AB16" s="36">
+      <c r="AB16" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2231,7 +2178,7 @@
       </c>
       <c r="AF16" s="20"/>
       <c r="AG16" s="20"/>
-      <c r="AH16" s="36">
+      <c r="AH16" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2244,7 +2191,7 @@
       </c>
       <c r="AL16" s="20"/>
       <c r="AM16" s="20"/>
-      <c r="AN16" s="36">
+      <c r="AN16" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -2257,7 +2204,7 @@
       </c>
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
-      <c r="AT16" s="36">
+      <c r="AT16" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2270,7 +2217,7 @@
       </c>
       <c r="AX16" s="20"/>
       <c r="AY16" s="20"/>
-      <c r="AZ16" s="36">
+      <c r="AZ16" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -2283,7 +2230,7 @@
       </c>
       <c r="BD16" s="20"/>
       <c r="BE16" s="20"/>
-      <c r="BF16" s="36">
+      <c r="BF16" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2296,7 +2243,7 @@
       </c>
       <c r="BJ16" s="20"/>
       <c r="BK16" s="20"/>
-      <c r="BL16" s="36">
+      <c r="BL16" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -2309,7 +2256,7 @@
       </c>
       <c r="BP16" s="20"/>
       <c r="BQ16" s="20"/>
-      <c r="BR16" s="36">
+      <c r="BR16" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -2322,7 +2269,7 @@
       </c>
       <c r="BV16" s="20"/>
       <c r="BW16" s="20"/>
-      <c r="BX16" s="36">
+      <c r="BX16" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -2335,7 +2282,7 @@
       </c>
       <c r="CB16" s="20"/>
       <c r="CC16" s="20"/>
-      <c r="CD16" s="36">
+      <c r="CD16" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -2348,7 +2295,7 @@
       </c>
       <c r="CH16" s="20"/>
       <c r="CI16" s="20"/>
-      <c r="CJ16" s="36">
+      <c r="CJ16" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -2372,7 +2319,7 @@
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
-      <c r="J17" s="36">
+      <c r="J17" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2385,7 +2332,7 @@
       </c>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
-      <c r="P17" s="36">
+      <c r="P17" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2398,7 +2345,7 @@
       </c>
       <c r="T17" s="20"/>
       <c r="U17" s="20"/>
-      <c r="V17" s="36">
+      <c r="V17" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2411,7 +2358,7 @@
       </c>
       <c r="Z17" s="20"/>
       <c r="AA17" s="20"/>
-      <c r="AB17" s="36">
+      <c r="AB17" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2424,7 +2371,7 @@
       </c>
       <c r="AF17" s="20"/>
       <c r="AG17" s="20"/>
-      <c r="AH17" s="36">
+      <c r="AH17" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2437,7 +2384,7 @@
       </c>
       <c r="AL17" s="20"/>
       <c r="AM17" s="20"/>
-      <c r="AN17" s="36">
+      <c r="AN17" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -2450,7 +2397,7 @@
       </c>
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
-      <c r="AT17" s="36">
+      <c r="AT17" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2463,7 +2410,7 @@
       </c>
       <c r="AX17" s="20"/>
       <c r="AY17" s="20"/>
-      <c r="AZ17" s="36">
+      <c r="AZ17" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -2476,7 +2423,7 @@
       </c>
       <c r="BD17" s="20"/>
       <c r="BE17" s="20"/>
-      <c r="BF17" s="36">
+      <c r="BF17" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2489,7 +2436,7 @@
       </c>
       <c r="BJ17" s="20"/>
       <c r="BK17" s="20"/>
-      <c r="BL17" s="36">
+      <c r="BL17" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -2502,7 +2449,7 @@
       </c>
       <c r="BP17" s="20"/>
       <c r="BQ17" s="20"/>
-      <c r="BR17" s="36">
+      <c r="BR17" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -2515,7 +2462,7 @@
       </c>
       <c r="BV17" s="20"/>
       <c r="BW17" s="20"/>
-      <c r="BX17" s="36">
+      <c r="BX17" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -2528,7 +2475,7 @@
       </c>
       <c r="CB17" s="20"/>
       <c r="CC17" s="20"/>
-      <c r="CD17" s="36">
+      <c r="CD17" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -2541,7 +2488,7 @@
       </c>
       <c r="CH17" s="20"/>
       <c r="CI17" s="20"/>
-      <c r="CJ17" s="36">
+      <c r="CJ17" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -2565,7 +2512,7 @@
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
-      <c r="J18" s="36">
+      <c r="J18" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2578,7 +2525,7 @@
       </c>
       <c r="N18" s="20"/>
       <c r="O18" s="20"/>
-      <c r="P18" s="36">
+      <c r="P18" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2591,7 +2538,7 @@
       </c>
       <c r="T18" s="20"/>
       <c r="U18" s="20"/>
-      <c r="V18" s="36">
+      <c r="V18" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2604,7 +2551,7 @@
       </c>
       <c r="Z18" s="20"/>
       <c r="AA18" s="20"/>
-      <c r="AB18" s="36">
+      <c r="AB18" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2617,7 +2564,7 @@
       </c>
       <c r="AF18" s="20"/>
       <c r="AG18" s="20"/>
-      <c r="AH18" s="36">
+      <c r="AH18" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2630,7 +2577,7 @@
       </c>
       <c r="AL18" s="20"/>
       <c r="AM18" s="20"/>
-      <c r="AN18" s="36">
+      <c r="AN18" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -2643,7 +2590,7 @@
       </c>
       <c r="AR18" s="20"/>
       <c r="AS18" s="20"/>
-      <c r="AT18" s="36">
+      <c r="AT18" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2656,7 +2603,7 @@
       </c>
       <c r="AX18" s="20"/>
       <c r="AY18" s="20"/>
-      <c r="AZ18" s="36">
+      <c r="AZ18" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -2669,7 +2616,7 @@
       </c>
       <c r="BD18" s="20"/>
       <c r="BE18" s="20"/>
-      <c r="BF18" s="36">
+      <c r="BF18" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2682,7 +2629,7 @@
       </c>
       <c r="BJ18" s="20"/>
       <c r="BK18" s="20"/>
-      <c r="BL18" s="36">
+      <c r="BL18" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -2695,7 +2642,7 @@
       </c>
       <c r="BP18" s="20"/>
       <c r="BQ18" s="20"/>
-      <c r="BR18" s="36">
+      <c r="BR18" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -2708,7 +2655,7 @@
       </c>
       <c r="BV18" s="20"/>
       <c r="BW18" s="20"/>
-      <c r="BX18" s="36">
+      <c r="BX18" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -2721,7 +2668,7 @@
       </c>
       <c r="CB18" s="20"/>
       <c r="CC18" s="20"/>
-      <c r="CD18" s="36">
+      <c r="CD18" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -2734,7 +2681,7 @@
       </c>
       <c r="CH18" s="20"/>
       <c r="CI18" s="20"/>
-      <c r="CJ18" s="36">
+      <c r="CJ18" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -2758,7 +2705,7 @@
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="36">
+      <c r="J19" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2771,7 +2718,7 @@
       </c>
       <c r="N19" s="20"/>
       <c r="O19" s="20"/>
-      <c r="P19" s="36">
+      <c r="P19" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2784,7 +2731,7 @@
       </c>
       <c r="T19" s="20"/>
       <c r="U19" s="20"/>
-      <c r="V19" s="36">
+      <c r="V19" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2797,7 +2744,7 @@
       </c>
       <c r="Z19" s="20"/>
       <c r="AA19" s="20"/>
-      <c r="AB19" s="36">
+      <c r="AB19" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2810,7 +2757,7 @@
       </c>
       <c r="AF19" s="20"/>
       <c r="AG19" s="20"/>
-      <c r="AH19" s="36">
+      <c r="AH19" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2823,7 +2770,7 @@
       </c>
       <c r="AL19" s="20"/>
       <c r="AM19" s="20"/>
-      <c r="AN19" s="36">
+      <c r="AN19" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -2836,7 +2783,7 @@
       </c>
       <c r="AR19" s="20"/>
       <c r="AS19" s="20"/>
-      <c r="AT19" s="36">
+      <c r="AT19" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2849,7 +2796,7 @@
       </c>
       <c r="AX19" s="20"/>
       <c r="AY19" s="20"/>
-      <c r="AZ19" s="36">
+      <c r="AZ19" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -2862,7 +2809,7 @@
       </c>
       <c r="BD19" s="20"/>
       <c r="BE19" s="20"/>
-      <c r="BF19" s="36">
+      <c r="BF19" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -2875,7 +2822,7 @@
       </c>
       <c r="BJ19" s="20"/>
       <c r="BK19" s="20"/>
-      <c r="BL19" s="36">
+      <c r="BL19" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -2888,7 +2835,7 @@
       </c>
       <c r="BP19" s="20"/>
       <c r="BQ19" s="20"/>
-      <c r="BR19" s="36">
+      <c r="BR19" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -2901,7 +2848,7 @@
       </c>
       <c r="BV19" s="20"/>
       <c r="BW19" s="20"/>
-      <c r="BX19" s="36">
+      <c r="BX19" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -2914,7 +2861,7 @@
       </c>
       <c r="CB19" s="20"/>
       <c r="CC19" s="20"/>
-      <c r="CD19" s="36">
+      <c r="CD19" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -2927,7 +2874,7 @@
       </c>
       <c r="CH19" s="20"/>
       <c r="CI19" s="20"/>
-      <c r="CJ19" s="36">
+      <c r="CJ19" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -2951,7 +2898,7 @@
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
-      <c r="J20" s="36">
+      <c r="J20" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2964,7 +2911,7 @@
       </c>
       <c r="N20" s="20"/>
       <c r="O20" s="20"/>
-      <c r="P20" s="36">
+      <c r="P20" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2977,7 +2924,7 @@
       </c>
       <c r="T20" s="20"/>
       <c r="U20" s="20"/>
-      <c r="V20" s="36">
+      <c r="V20" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2990,7 +2937,7 @@
       </c>
       <c r="Z20" s="20"/>
       <c r="AA20" s="20"/>
-      <c r="AB20" s="36">
+      <c r="AB20" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3003,7 +2950,7 @@
       </c>
       <c r="AF20" s="20"/>
       <c r="AG20" s="20"/>
-      <c r="AH20" s="36">
+      <c r="AH20" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3016,7 +2963,7 @@
       </c>
       <c r="AL20" s="20"/>
       <c r="AM20" s="20"/>
-      <c r="AN20" s="36">
+      <c r="AN20" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3029,7 +2976,7 @@
       </c>
       <c r="AR20" s="20"/>
       <c r="AS20" s="20"/>
-      <c r="AT20" s="36">
+      <c r="AT20" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3042,7 +2989,7 @@
       </c>
       <c r="AX20" s="20"/>
       <c r="AY20" s="20"/>
-      <c r="AZ20" s="36">
+      <c r="AZ20" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -3055,7 +3002,7 @@
       </c>
       <c r="BD20" s="20"/>
       <c r="BE20" s="20"/>
-      <c r="BF20" s="36">
+      <c r="BF20" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -3068,7 +3015,7 @@
       </c>
       <c r="BJ20" s="20"/>
       <c r="BK20" s="20"/>
-      <c r="BL20" s="36">
+      <c r="BL20" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -3081,7 +3028,7 @@
       </c>
       <c r="BP20" s="20"/>
       <c r="BQ20" s="20"/>
-      <c r="BR20" s="36">
+      <c r="BR20" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3094,7 +3041,7 @@
       </c>
       <c r="BV20" s="20"/>
       <c r="BW20" s="20"/>
-      <c r="BX20" s="36">
+      <c r="BX20" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3107,7 +3054,7 @@
       </c>
       <c r="CB20" s="20"/>
       <c r="CC20" s="20"/>
-      <c r="CD20" s="36">
+      <c r="CD20" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -3120,7 +3067,7 @@
       </c>
       <c r="CH20" s="20"/>
       <c r="CI20" s="20"/>
-      <c r="CJ20" s="36">
+      <c r="CJ20" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -3144,7 +3091,7 @@
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
-      <c r="J21" s="36">
+      <c r="J21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3157,7 +3104,7 @@
       </c>
       <c r="N21" s="20"/>
       <c r="O21" s="20"/>
-      <c r="P21" s="36">
+      <c r="P21" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3170,7 +3117,7 @@
       </c>
       <c r="T21" s="20"/>
       <c r="U21" s="20"/>
-      <c r="V21" s="36">
+      <c r="V21" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3183,7 +3130,7 @@
       </c>
       <c r="Z21" s="20"/>
       <c r="AA21" s="20"/>
-      <c r="AB21" s="36">
+      <c r="AB21" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3196,7 +3143,7 @@
       </c>
       <c r="AF21" s="20"/>
       <c r="AG21" s="20"/>
-      <c r="AH21" s="36">
+      <c r="AH21" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3209,7 +3156,7 @@
       </c>
       <c r="AL21" s="20"/>
       <c r="AM21" s="20"/>
-      <c r="AN21" s="36">
+      <c r="AN21" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3222,7 +3169,7 @@
       </c>
       <c r="AR21" s="20"/>
       <c r="AS21" s="20"/>
-      <c r="AT21" s="36">
+      <c r="AT21" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3235,7 +3182,7 @@
       </c>
       <c r="AX21" s="20"/>
       <c r="AY21" s="20"/>
-      <c r="AZ21" s="36">
+      <c r="AZ21" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -3248,7 +3195,7 @@
       </c>
       <c r="BD21" s="20"/>
       <c r="BE21" s="20"/>
-      <c r="BF21" s="36">
+      <c r="BF21" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -3261,7 +3208,7 @@
       </c>
       <c r="BJ21" s="20"/>
       <c r="BK21" s="20"/>
-      <c r="BL21" s="36">
+      <c r="BL21" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -3274,7 +3221,7 @@
       </c>
       <c r="BP21" s="20"/>
       <c r="BQ21" s="20"/>
-      <c r="BR21" s="36">
+      <c r="BR21" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3287,7 +3234,7 @@
       </c>
       <c r="BV21" s="20"/>
       <c r="BW21" s="20"/>
-      <c r="BX21" s="36">
+      <c r="BX21" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3300,7 +3247,7 @@
       </c>
       <c r="CB21" s="20"/>
       <c r="CC21" s="20"/>
-      <c r="CD21" s="36">
+      <c r="CD21" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -3313,7 +3260,7 @@
       </c>
       <c r="CH21" s="20"/>
       <c r="CI21" s="20"/>
-      <c r="CJ21" s="36">
+      <c r="CJ21" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -3337,7 +3284,7 @@
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
-      <c r="J22" s="36">
+      <c r="J22" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3350,7 +3297,7 @@
       </c>
       <c r="N22" s="20"/>
       <c r="O22" s="20"/>
-      <c r="P22" s="36">
+      <c r="P22" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3363,7 +3310,7 @@
       </c>
       <c r="T22" s="20"/>
       <c r="U22" s="20"/>
-      <c r="V22" s="36">
+      <c r="V22" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3376,7 +3323,7 @@
       </c>
       <c r="Z22" s="20"/>
       <c r="AA22" s="20"/>
-      <c r="AB22" s="36">
+      <c r="AB22" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3389,7 +3336,7 @@
       </c>
       <c r="AF22" s="20"/>
       <c r="AG22" s="20"/>
-      <c r="AH22" s="36">
+      <c r="AH22" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3402,7 +3349,7 @@
       </c>
       <c r="AL22" s="20"/>
       <c r="AM22" s="20"/>
-      <c r="AN22" s="36">
+      <c r="AN22" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3415,7 +3362,7 @@
       </c>
       <c r="AR22" s="20"/>
       <c r="AS22" s="20"/>
-      <c r="AT22" s="36">
+      <c r="AT22" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3428,7 +3375,7 @@
       </c>
       <c r="AX22" s="20"/>
       <c r="AY22" s="20"/>
-      <c r="AZ22" s="36">
+      <c r="AZ22" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -3441,7 +3388,7 @@
       </c>
       <c r="BD22" s="20"/>
       <c r="BE22" s="20"/>
-      <c r="BF22" s="36">
+      <c r="BF22" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -3454,7 +3401,7 @@
       </c>
       <c r="BJ22" s="20"/>
       <c r="BK22" s="20"/>
-      <c r="BL22" s="36">
+      <c r="BL22" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -3467,7 +3414,7 @@
       </c>
       <c r="BP22" s="20"/>
       <c r="BQ22" s="20"/>
-      <c r="BR22" s="36">
+      <c r="BR22" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3480,7 +3427,7 @@
       </c>
       <c r="BV22" s="20"/>
       <c r="BW22" s="20"/>
-      <c r="BX22" s="36">
+      <c r="BX22" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3493,7 +3440,7 @@
       </c>
       <c r="CB22" s="20"/>
       <c r="CC22" s="20"/>
-      <c r="CD22" s="36">
+      <c r="CD22" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -3506,7 +3453,7 @@
       </c>
       <c r="CH22" s="20"/>
       <c r="CI22" s="20"/>
-      <c r="CJ22" s="36">
+      <c r="CJ22" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -3530,7 +3477,7 @@
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
-      <c r="J23" s="36">
+      <c r="J23" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3543,7 +3490,7 @@
       </c>
       <c r="N23" s="20"/>
       <c r="O23" s="20"/>
-      <c r="P23" s="36">
+      <c r="P23" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3556,7 +3503,7 @@
       </c>
       <c r="T23" s="20"/>
       <c r="U23" s="20"/>
-      <c r="V23" s="36">
+      <c r="V23" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3569,7 +3516,7 @@
       </c>
       <c r="Z23" s="20"/>
       <c r="AA23" s="20"/>
-      <c r="AB23" s="36">
+      <c r="AB23" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3582,7 +3529,7 @@
       </c>
       <c r="AF23" s="20"/>
       <c r="AG23" s="20"/>
-      <c r="AH23" s="36">
+      <c r="AH23" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3595,7 +3542,7 @@
       </c>
       <c r="AL23" s="20"/>
       <c r="AM23" s="20"/>
-      <c r="AN23" s="36">
+      <c r="AN23" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3608,7 +3555,7 @@
       </c>
       <c r="AR23" s="20"/>
       <c r="AS23" s="20"/>
-      <c r="AT23" s="36">
+      <c r="AT23" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3621,7 +3568,7 @@
       </c>
       <c r="AX23" s="20"/>
       <c r="AY23" s="20"/>
-      <c r="AZ23" s="36">
+      <c r="AZ23" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -3634,7 +3581,7 @@
       </c>
       <c r="BD23" s="20"/>
       <c r="BE23" s="20"/>
-      <c r="BF23" s="36">
+      <c r="BF23" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -3647,7 +3594,7 @@
       </c>
       <c r="BJ23" s="20"/>
       <c r="BK23" s="20"/>
-      <c r="BL23" s="36">
+      <c r="BL23" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -3660,7 +3607,7 @@
       </c>
       <c r="BP23" s="20"/>
       <c r="BQ23" s="20"/>
-      <c r="BR23" s="36">
+      <c r="BR23" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3673,7 +3620,7 @@
       </c>
       <c r="BV23" s="20"/>
       <c r="BW23" s="20"/>
-      <c r="BX23" s="36">
+      <c r="BX23" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3686,7 +3633,7 @@
       </c>
       <c r="CB23" s="20"/>
       <c r="CC23" s="20"/>
-      <c r="CD23" s="36">
+      <c r="CD23" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -3699,7 +3646,7 @@
       </c>
       <c r="CH23" s="20"/>
       <c r="CI23" s="20"/>
-      <c r="CJ23" s="36">
+      <c r="CJ23" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -3723,7 +3670,7 @@
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
-      <c r="J24" s="36">
+      <c r="J24" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3736,7 +3683,7 @@
       </c>
       <c r="N24" s="20"/>
       <c r="O24" s="20"/>
-      <c r="P24" s="36">
+      <c r="P24" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3749,7 +3696,7 @@
       </c>
       <c r="T24" s="20"/>
       <c r="U24" s="20"/>
-      <c r="V24" s="36">
+      <c r="V24" s="33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3762,7 +3709,7 @@
       </c>
       <c r="Z24" s="20"/>
       <c r="AA24" s="20"/>
-      <c r="AB24" s="36">
+      <c r="AB24" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3775,7 +3722,7 @@
       </c>
       <c r="AF24" s="20"/>
       <c r="AG24" s="20"/>
-      <c r="AH24" s="36">
+      <c r="AH24" s="33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3788,7 +3735,7 @@
       </c>
       <c r="AL24" s="20"/>
       <c r="AM24" s="20"/>
-      <c r="AN24" s="36">
+      <c r="AN24" s="33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3801,7 +3748,7 @@
       </c>
       <c r="AR24" s="20"/>
       <c r="AS24" s="20"/>
-      <c r="AT24" s="36">
+      <c r="AT24" s="33">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -3814,7 +3761,7 @@
       </c>
       <c r="AX24" s="20"/>
       <c r="AY24" s="20"/>
-      <c r="AZ24" s="36">
+      <c r="AZ24" s="33">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -3827,7 +3774,7 @@
       </c>
       <c r="BD24" s="20"/>
       <c r="BE24" s="20"/>
-      <c r="BF24" s="36">
+      <c r="BF24" s="33">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -3840,7 +3787,7 @@
       </c>
       <c r="BJ24" s="20"/>
       <c r="BK24" s="20"/>
-      <c r="BL24" s="36">
+      <c r="BL24" s="33">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -3853,7 +3800,7 @@
       </c>
       <c r="BP24" s="20"/>
       <c r="BQ24" s="20"/>
-      <c r="BR24" s="36">
+      <c r="BR24" s="33">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3866,7 +3813,7 @@
       </c>
       <c r="BV24" s="20"/>
       <c r="BW24" s="20"/>
-      <c r="BX24" s="36">
+      <c r="BX24" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3879,7 +3826,7 @@
       </c>
       <c r="CB24" s="20"/>
       <c r="CC24" s="20"/>
-      <c r="CD24" s="36">
+      <c r="CD24" s="33">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -3892,7 +3839,7 @@
       </c>
       <c r="CH24" s="20"/>
       <c r="CI24" s="20"/>
-      <c r="CJ24" s="36">
+      <c r="CJ24" s="33">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -3916,7 +3863,7 @@
       </c>
       <c r="H25" s="23"/>
       <c r="I25" s="23"/>
-      <c r="J25" s="37">
+      <c r="J25" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3929,7 +3876,7 @@
       </c>
       <c r="N25" s="23"/>
       <c r="O25" s="23"/>
-      <c r="P25" s="37">
+      <c r="P25" s="34">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3942,7 +3889,7 @@
       </c>
       <c r="T25" s="23"/>
       <c r="U25" s="23"/>
-      <c r="V25" s="37">
+      <c r="V25" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3955,7 +3902,7 @@
       </c>
       <c r="Z25" s="23"/>
       <c r="AA25" s="23"/>
-      <c r="AB25" s="37">
+      <c r="AB25" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3968,7 +3915,7 @@
       </c>
       <c r="AF25" s="23"/>
       <c r="AG25" s="23"/>
-      <c r="AH25" s="37">
+      <c r="AH25" s="34">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3981,7 +3928,7 @@
       </c>
       <c r="AL25" s="23"/>
       <c r="AM25" s="23"/>
-      <c r="AN25" s="37">
+      <c r="AN25" s="34">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3994,7 +3941,7 @@
       </c>
       <c r="AR25" s="23"/>
       <c r="AS25" s="23"/>
-      <c r="AT25" s="37">
+      <c r="AT25" s="34">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -4007,7 +3954,7 @@
       </c>
       <c r="AX25" s="23"/>
       <c r="AY25" s="23"/>
-      <c r="AZ25" s="37">
+      <c r="AZ25" s="34">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -4020,7 +3967,7 @@
       </c>
       <c r="BD25" s="23"/>
       <c r="BE25" s="23"/>
-      <c r="BF25" s="37">
+      <c r="BF25" s="34">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -4033,7 +3980,7 @@
       </c>
       <c r="BJ25" s="23"/>
       <c r="BK25" s="23"/>
-      <c r="BL25" s="37">
+      <c r="BL25" s="34">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -4046,7 +3993,7 @@
       </c>
       <c r="BP25" s="23"/>
       <c r="BQ25" s="23"/>
-      <c r="BR25" s="37">
+      <c r="BR25" s="34">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -4059,7 +4006,7 @@
       </c>
       <c r="BV25" s="23"/>
       <c r="BW25" s="23"/>
-      <c r="BX25" s="37">
+      <c r="BX25" s="34">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -4072,7 +4019,7 @@
       </c>
       <c r="CB25" s="23"/>
       <c r="CC25" s="23"/>
-      <c r="CD25" s="37">
+      <c r="CD25" s="34">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
@@ -4085,7 +4032,7 @@
       </c>
       <c r="CH25" s="23"/>
       <c r="CI25" s="23"/>
-      <c r="CJ25" s="37">
+      <c r="CJ25" s="34">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -4104,12 +4051,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="38">
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="35">
         <f>SUM(J14:J25)</f>
         <v>0</v>
       </c>
@@ -4117,12 +4064,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M26" s="42" t="s">
+      <c r="M26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="38">
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="35">
         <f>SUM(P14:P25)</f>
         <v>0</v>
       </c>
@@ -4130,12 +4077,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S26" s="42" t="s">
+      <c r="S26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="38">
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="35">
         <f>SUM(V14:V25)</f>
         <v>0</v>
       </c>
@@ -4143,12 +4090,12 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y26" s="42" t="s">
+      <c r="Y26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="Z26" s="43"/>
-      <c r="AA26" s="43"/>
-      <c r="AB26" s="38">
+      <c r="Z26" s="37"/>
+      <c r="AA26" s="37"/>
+      <c r="AB26" s="35">
         <f>SUM(AB14:AB25)</f>
         <v>0</v>
       </c>
@@ -4156,12 +4103,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="42" t="s">
+      <c r="AE26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AF26" s="43"/>
-      <c r="AG26" s="43"/>
-      <c r="AH26" s="38">
+      <c r="AF26" s="37"/>
+      <c r="AG26" s="37"/>
+      <c r="AH26" s="35">
         <f>SUM(AH14:AH25)</f>
         <v>0</v>
       </c>
@@ -4169,12 +4116,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AK26" s="42" t="s">
+      <c r="AK26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AL26" s="43"/>
-      <c r="AM26" s="43"/>
-      <c r="AN26" s="38">
+      <c r="AL26" s="37"/>
+      <c r="AM26" s="37"/>
+      <c r="AN26" s="35">
         <f>SUM(AN14:AN25)</f>
         <v>0</v>
       </c>
@@ -4182,12 +4129,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AQ26" s="42" t="s">
+      <c r="AQ26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AR26" s="43"/>
-      <c r="AS26" s="43"/>
-      <c r="AT26" s="38">
+      <c r="AR26" s="37"/>
+      <c r="AS26" s="37"/>
+      <c r="AT26" s="35">
         <f>SUM(AT14:AT25)</f>
         <v>0</v>
       </c>
@@ -4195,12 +4142,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AW26" s="42" t="s">
+      <c r="AW26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AX26" s="43"/>
-      <c r="AY26" s="43"/>
-      <c r="AZ26" s="38">
+      <c r="AX26" s="37"/>
+      <c r="AY26" s="37"/>
+      <c r="AZ26" s="35">
         <f>SUM(AZ14:AZ25)</f>
         <v>0</v>
       </c>
@@ -4208,12 +4155,12 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="BC26" s="42" t="s">
+      <c r="BC26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="BD26" s="43"/>
-      <c r="BE26" s="43"/>
-      <c r="BF26" s="38">
+      <c r="BD26" s="37"/>
+      <c r="BE26" s="37"/>
+      <c r="BF26" s="35">
         <f>SUM(BF14:BF25)</f>
         <v>0</v>
       </c>
@@ -4221,12 +4168,12 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="BI26" s="42" t="s">
+      <c r="BI26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="BJ26" s="43"/>
-      <c r="BK26" s="43"/>
-      <c r="BL26" s="38">
+      <c r="BJ26" s="37"/>
+      <c r="BK26" s="37"/>
+      <c r="BL26" s="35">
         <f>SUM(BL14:BL25)</f>
         <v>0</v>
       </c>
@@ -4234,12 +4181,12 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="BO26" s="42" t="s">
+      <c r="BO26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="BP26" s="43"/>
-      <c r="BQ26" s="43"/>
-      <c r="BR26" s="38">
+      <c r="BP26" s="37"/>
+      <c r="BQ26" s="37"/>
+      <c r="BR26" s="35">
         <f>SUM(BR14:BR25)</f>
         <v>0</v>
       </c>
@@ -4247,12 +4194,12 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="BU26" s="42" t="s">
+      <c r="BU26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="BV26" s="43"/>
-      <c r="BW26" s="43"/>
-      <c r="BX26" s="38">
+      <c r="BV26" s="37"/>
+      <c r="BW26" s="37"/>
+      <c r="BX26" s="35">
         <f>SUM(BX14:BX25)</f>
         <v>0</v>
       </c>
@@ -4260,12 +4207,12 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="CA26" s="42" t="s">
+      <c r="CA26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="CB26" s="43"/>
-      <c r="CC26" s="43"/>
-      <c r="CD26" s="38">
+      <c r="CB26" s="37"/>
+      <c r="CC26" s="37"/>
+      <c r="CD26" s="35">
         <f>SUM(CD14:CD25)</f>
         <v>0</v>
       </c>
@@ -4273,12 +4220,12 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="CG26" s="42" t="s">
+      <c r="CG26" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="CH26" s="43"/>
-      <c r="CI26" s="43"/>
-      <c r="CJ26" s="38">
+      <c r="CH26" s="37"/>
+      <c r="CI26" s="37"/>
+      <c r="CJ26" s="35">
         <f>SUM(CJ14:CJ25)</f>
         <v>0</v>
       </c>
@@ -4288,43 +4235,30 @@
       </c>
     </row>
     <row r="27" spans="2:89" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B27" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="26">
+        <f>SUM(E14:E26)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="27"/>
     </row>
-    <row r="28" spans="2:89" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="29">
-        <f>SUM(E14:E27)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="30"/>
-    </row>
+    <row r="28" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="CG26:CI26"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="AW26:AY26"/>
-    <mergeCell ref="BC26:BE26"/>
-    <mergeCell ref="BI26:BK26"/>
-    <mergeCell ref="BO26:BQ26"/>
-    <mergeCell ref="BU26:BW26"/>
-    <mergeCell ref="CA26:CC26"/>
+    <mergeCell ref="AE12:AI12"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="S12:W12"/>
+    <mergeCell ref="Y12:AC12"/>
     <mergeCell ref="BU12:BY12"/>
     <mergeCell ref="CA12:CE12"/>
     <mergeCell ref="CG12:CK12"/>
@@ -4341,12 +4275,14 @@
     <mergeCell ref="BC12:BG12"/>
     <mergeCell ref="BI12:BM12"/>
     <mergeCell ref="BO12:BS12"/>
-    <mergeCell ref="AE12:AI12"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="S12:W12"/>
-    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="CG26:CI26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="AW26:AY26"/>
+    <mergeCell ref="BC26:BE26"/>
+    <mergeCell ref="BI26:BK26"/>
+    <mergeCell ref="BO26:BQ26"/>
+    <mergeCell ref="BU26:BW26"/>
+    <mergeCell ref="CA26:CC26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>